<commit_message>
2024 needs to be checked some issues were found
</commit_message>
<xml_diff>
--- a/data/raw_data/2023/permits-by-sector-2023.xlsx
+++ b/data/raw_data/2023/permits-by-sector-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://djei.cloud.gov.ie/apps/eDocs/S/ENT218/Files/ENT218-001-2023/Web Stats 2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Drive\ESTUDOS DATA SCIENCE\ie-employment-permit\data\raw_data\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48F56E3B-8196-45CA-921A-8744201CA762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23DF618-A355-4609-9B86-7A181993AF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{27EE0F96-6733-41FE-8F6D-14C706DBB3F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{27EE0F96-6733-41FE-8F6D-14C706DBB3F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Grand Total</t>
   </si>
@@ -80,9 +79,6 @@
   </si>
   <si>
     <t>Economic Sector</t>
-  </si>
-  <si>
-    <t>Issued</t>
   </si>
   <si>
     <t>A - Agriculture, Forestry &amp; Fishing</t>
@@ -166,7 +162,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -241,32 +237,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -582,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F6C83F-B704-4E77-94A1-6D38B78109DC}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,403 +584,407 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7" t="s">
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>15</v>
+      <c r="B3" s="3">
+        <v>1385</v>
+      </c>
+      <c r="C3" s="3">
+        <v>87</v>
+      </c>
+      <c r="D3" s="3">
+        <v>83</v>
+      </c>
+      <c r="E3" s="3">
+        <v>469</v>
+      </c>
+      <c r="F3" s="3">
+        <v>253</v>
+      </c>
+      <c r="G3" s="3">
+        <v>91</v>
+      </c>
+      <c r="H3" s="3">
+        <v>56</v>
+      </c>
+      <c r="I3" s="3">
+        <v>62</v>
+      </c>
+      <c r="J3" s="3">
+        <v>56</v>
+      </c>
+      <c r="K3" s="3">
+        <v>42</v>
+      </c>
+      <c r="L3" s="3">
+        <v>43</v>
+      </c>
+      <c r="M3" s="3">
+        <v>66</v>
+      </c>
+      <c r="N3" s="3">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="10">
-        <v>30981</v>
-      </c>
-      <c r="C4" s="10">
-        <v>2527</v>
-      </c>
-      <c r="D4" s="10">
-        <v>2192</v>
-      </c>
-      <c r="E4" s="10">
-        <v>2546</v>
-      </c>
-      <c r="F4" s="10">
-        <v>2179</v>
-      </c>
-      <c r="G4" s="10">
-        <v>2758</v>
-      </c>
-      <c r="H4" s="10">
-        <v>3138</v>
-      </c>
-      <c r="I4" s="10">
-        <v>3031</v>
-      </c>
-      <c r="J4" s="10">
-        <v>2411</v>
-      </c>
-      <c r="K4" s="10">
-        <v>2203</v>
-      </c>
-      <c r="L4" s="10">
-        <v>2544</v>
-      </c>
-      <c r="M4" s="10">
-        <v>3005</v>
-      </c>
-      <c r="N4" s="10">
-        <v>2447</v>
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="3">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="3">
+        <v>4</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2</v>
+      </c>
+      <c r="J4" s="3">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3">
+        <v>7</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3">
-        <v>1385</v>
+        <v>766</v>
       </c>
       <c r="C5" s="3">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="D5" s="3">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="E5" s="3">
-        <v>469</v>
+        <v>58</v>
       </c>
       <c r="F5" s="3">
-        <v>253</v>
+        <v>44</v>
       </c>
       <c r="G5" s="3">
+        <v>78</v>
+      </c>
+      <c r="H5" s="3">
+        <v>78</v>
+      </c>
+      <c r="I5" s="3">
+        <v>77</v>
+      </c>
+      <c r="J5" s="3">
+        <v>50</v>
+      </c>
+      <c r="K5" s="3">
+        <v>56</v>
+      </c>
+      <c r="L5" s="3">
+        <v>57</v>
+      </c>
+      <c r="M5" s="3">
         <v>91</v>
       </c>
-      <c r="H5" s="3">
-        <v>56</v>
-      </c>
-      <c r="I5" s="3">
-        <v>62</v>
-      </c>
-      <c r="J5" s="3">
-        <v>56</v>
-      </c>
-      <c r="K5" s="3">
-        <v>42</v>
-      </c>
-      <c r="L5" s="3">
-        <v>43</v>
-      </c>
-      <c r="M5" s="3">
-        <v>66</v>
-      </c>
       <c r="N5" s="3">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3">
-        <v>30</v>
+        <v>877</v>
       </c>
       <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="D6" s="3">
+        <v>47</v>
+      </c>
+      <c r="E6" s="3">
+        <v>41</v>
+      </c>
       <c r="F6" s="3">
-        <v>8</v>
-      </c>
-      <c r="G6" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="G6" s="3">
+        <v>90</v>
+      </c>
       <c r="H6" s="3">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="I6" s="3">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="J6" s="3">
-        <v>3</v>
+        <v>91</v>
       </c>
       <c r="K6" s="3">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="L6" s="3">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="M6" s="3">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="N6" s="3">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3">
-        <v>766</v>
+        <v>845</v>
       </c>
       <c r="C7" s="3">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="D7" s="3">
+        <v>42</v>
+      </c>
+      <c r="E7" s="3">
+        <v>51</v>
+      </c>
+      <c r="F7" s="3">
+        <v>62</v>
+      </c>
+      <c r="G7" s="3">
+        <v>86</v>
+      </c>
+      <c r="H7" s="3">
+        <v>137</v>
+      </c>
+      <c r="I7" s="3">
+        <v>158</v>
+      </c>
+      <c r="J7" s="3">
+        <v>55</v>
+      </c>
+      <c r="K7" s="3">
+        <v>58</v>
+      </c>
+      <c r="L7" s="3">
         <v>45</v>
       </c>
-      <c r="E7" s="3">
-        <v>58</v>
-      </c>
-      <c r="F7" s="3">
-        <v>44</v>
-      </c>
-      <c r="G7" s="3">
-        <v>78</v>
-      </c>
-      <c r="H7" s="3">
-        <v>78</v>
-      </c>
-      <c r="I7" s="3">
-        <v>77</v>
-      </c>
-      <c r="J7" s="3">
-        <v>50</v>
-      </c>
-      <c r="K7" s="3">
-        <v>56</v>
-      </c>
-      <c r="L7" s="3">
-        <v>57</v>
-      </c>
       <c r="M7" s="3">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="N7" s="3">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3">
+        <v>268</v>
+      </c>
+      <c r="C8" s="3">
+        <v>23</v>
+      </c>
+      <c r="D8" s="3">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3">
         <v>19</v>
       </c>
-      <c r="B8" s="3">
-        <v>877</v>
-      </c>
-      <c r="C8" s="3">
-        <v>62</v>
-      </c>
-      <c r="D8" s="3">
-        <v>47</v>
-      </c>
-      <c r="E8" s="3">
-        <v>41</v>
-      </c>
       <c r="F8" s="3">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="G8" s="3">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="H8" s="3">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="I8" s="3">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="J8" s="3">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="K8" s="3">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="L8" s="3">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="M8" s="3">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="N8" s="3">
-        <v>53</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3">
-        <v>845</v>
+        <v>281</v>
       </c>
       <c r="C9" s="3">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="E9" s="3">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="F9" s="3">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="G9" s="3">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="H9" s="3">
-        <v>137</v>
+        <v>22</v>
       </c>
       <c r="I9" s="3">
-        <v>158</v>
+        <v>17</v>
       </c>
       <c r="J9" s="3">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="K9" s="3">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="L9" s="3">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="M9" s="3">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="N9" s="3">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="3">
-        <v>268</v>
+        <v>371</v>
       </c>
       <c r="C10" s="3">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3">
+        <v>13</v>
+      </c>
+      <c r="E10" s="3">
+        <v>27</v>
+      </c>
+      <c r="F10" s="3">
+        <v>15</v>
+      </c>
+      <c r="G10" s="3">
+        <v>35</v>
+      </c>
+      <c r="H10" s="3">
+        <v>46</v>
+      </c>
+      <c r="I10" s="3">
+        <v>56</v>
+      </c>
+      <c r="J10" s="3">
+        <v>45</v>
+      </c>
+      <c r="K10" s="3">
+        <v>32</v>
+      </c>
+      <c r="L10" s="3">
+        <v>34</v>
+      </c>
+      <c r="M10" s="3">
         <v>30</v>
-      </c>
-      <c r="E10" s="3">
-        <v>19</v>
-      </c>
-      <c r="F10" s="3">
-        <v>20</v>
-      </c>
-      <c r="G10" s="3">
-        <v>23</v>
-      </c>
-      <c r="H10" s="3">
-        <v>29</v>
-      </c>
-      <c r="I10" s="3">
-        <v>29</v>
-      </c>
-      <c r="J10" s="3">
-        <v>26</v>
-      </c>
-      <c r="K10" s="3">
-        <v>16</v>
-      </c>
-      <c r="L10" s="3">
-        <v>22</v>
-      </c>
-      <c r="M10" s="3">
-        <v>13</v>
       </c>
       <c r="N10" s="3">
         <v>18</v>
@@ -1001,805 +992,717 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3">
-        <v>281</v>
+        <v>87</v>
       </c>
       <c r="C11" s="3">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E11" s="3">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F11" s="3">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="G11" s="3">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="H11" s="3">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="I11" s="3">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J11" s="3">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="K11" s="3">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="L11" s="3">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="M11" s="3">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="N11" s="3">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3">
-        <v>371</v>
+        <v>1349</v>
       </c>
       <c r="C12" s="3">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="D12" s="3">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="E12" s="3">
-        <v>27</v>
+        <v>124</v>
       </c>
       <c r="F12" s="3">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="G12" s="3">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="H12" s="3">
-        <v>46</v>
+        <v>129</v>
       </c>
       <c r="I12" s="3">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="J12" s="3">
-        <v>45</v>
+        <v>111</v>
       </c>
       <c r="K12" s="3">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="L12" s="3">
-        <v>34</v>
+        <v>143</v>
       </c>
       <c r="M12" s="3">
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="N12" s="3">
-        <v>18</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3">
-        <v>87</v>
+        <v>294</v>
       </c>
       <c r="C13" s="3">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D13" s="3">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E13" s="3">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F13" s="3">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G13" s="3">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="H13" s="3">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="I13" s="3">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J13" s="3">
         <v>13</v>
       </c>
       <c r="K13" s="3">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="L13" s="3">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="M13" s="3">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="N13" s="3">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="3">
-        <v>1349</v>
+        <v>907</v>
       </c>
       <c r="C14" s="3">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="D14" s="3">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="E14" s="3">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="F14" s="3">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G14" s="3">
-        <v>136</v>
+        <v>54</v>
       </c>
       <c r="H14" s="3">
-        <v>129</v>
+        <v>83</v>
       </c>
       <c r="I14" s="3">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="J14" s="3">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="K14" s="3">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="L14" s="3">
-        <v>143</v>
+        <v>70</v>
       </c>
       <c r="M14" s="3">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="N14" s="3">
-        <v>99</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" s="3">
-        <v>294</v>
+        <v>2606</v>
       </c>
       <c r="C15" s="3">
-        <v>17</v>
+        <v>213</v>
       </c>
       <c r="D15" s="3">
-        <v>19</v>
+        <v>185</v>
       </c>
       <c r="E15" s="3">
-        <v>14</v>
+        <v>156</v>
       </c>
       <c r="F15" s="3">
-        <v>23</v>
+        <v>179</v>
       </c>
       <c r="G15" s="3">
-        <v>30</v>
+        <v>261</v>
       </c>
       <c r="H15" s="3">
-        <v>38</v>
+        <v>271</v>
       </c>
       <c r="I15" s="3">
-        <v>25</v>
+        <v>238</v>
       </c>
       <c r="J15" s="3">
-        <v>13</v>
+        <v>229</v>
       </c>
       <c r="K15" s="3">
-        <v>24</v>
+        <v>215</v>
       </c>
       <c r="L15" s="3">
-        <v>33</v>
+        <v>236</v>
       </c>
       <c r="M15" s="3">
-        <v>38</v>
+        <v>260</v>
       </c>
       <c r="N15" s="3">
-        <v>20</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3">
-        <v>907</v>
+        <v>5009</v>
       </c>
       <c r="C16" s="3">
-        <v>44</v>
+        <v>427</v>
       </c>
       <c r="D16" s="3">
-        <v>70</v>
+        <v>359</v>
       </c>
       <c r="E16" s="3">
-        <v>50</v>
+        <v>308</v>
       </c>
       <c r="F16" s="3">
-        <v>90</v>
+        <v>306</v>
       </c>
       <c r="G16" s="3">
-        <v>54</v>
+        <v>360</v>
       </c>
       <c r="H16" s="3">
-        <v>83</v>
+        <v>521</v>
       </c>
       <c r="I16" s="3">
-        <v>70</v>
+        <v>487</v>
       </c>
       <c r="J16" s="3">
-        <v>87</v>
+        <v>434</v>
       </c>
       <c r="K16" s="3">
-        <v>113</v>
+        <v>386</v>
       </c>
       <c r="L16" s="3">
-        <v>70</v>
+        <v>448</v>
       </c>
       <c r="M16" s="3">
-        <v>126</v>
+        <v>456</v>
       </c>
       <c r="N16" s="3">
-        <v>50</v>
+        <v>517</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" s="3">
-        <v>2606</v>
+        <v>2373</v>
       </c>
       <c r="C17" s="3">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="D17" s="3">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="E17" s="3">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="F17" s="3">
-        <v>179</v>
+        <v>130</v>
       </c>
       <c r="G17" s="3">
-        <v>261</v>
+        <v>197</v>
       </c>
       <c r="H17" s="3">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="I17" s="3">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="J17" s="3">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="K17" s="3">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="L17" s="3">
-        <v>236</v>
+        <v>202</v>
       </c>
       <c r="M17" s="3">
-        <v>260</v>
+        <v>233</v>
       </c>
       <c r="N17" s="3">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" s="3">
-        <v>5009</v>
+        <v>14</v>
       </c>
       <c r="C18" s="3">
-        <v>427</v>
+        <v>2</v>
       </c>
       <c r="D18" s="3">
-        <v>359</v>
+        <v>1</v>
       </c>
       <c r="E18" s="3">
-        <v>308</v>
-      </c>
-      <c r="F18" s="3">
-        <v>306</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F18" s="1"/>
       <c r="G18" s="3">
-        <v>360</v>
+        <v>1</v>
       </c>
       <c r="H18" s="3">
-        <v>521</v>
+        <v>1</v>
       </c>
       <c r="I18" s="3">
-        <v>487</v>
+        <v>1</v>
       </c>
       <c r="J18" s="3">
-        <v>434</v>
+        <v>1</v>
       </c>
       <c r="K18" s="3">
-        <v>386</v>
-      </c>
-      <c r="L18" s="3">
-        <v>448</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L18" s="1"/>
       <c r="M18" s="3">
-        <v>456</v>
-      </c>
-      <c r="N18" s="3">
-        <v>517</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="N18" s="1"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3">
-        <v>2373</v>
+        <v>1010</v>
       </c>
       <c r="C19" s="3">
-        <v>190</v>
+        <v>118</v>
       </c>
       <c r="D19" s="3">
-        <v>165</v>
+        <v>62</v>
       </c>
       <c r="E19" s="3">
-        <v>179</v>
+        <v>80</v>
       </c>
       <c r="F19" s="3">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="G19" s="3">
-        <v>197</v>
+        <v>73</v>
       </c>
       <c r="H19" s="3">
-        <v>252</v>
+        <v>118</v>
       </c>
       <c r="I19" s="3">
-        <v>224</v>
+        <v>103</v>
       </c>
       <c r="J19" s="3">
-        <v>225</v>
+        <v>83</v>
       </c>
       <c r="K19" s="3">
-        <v>219</v>
+        <v>61</v>
       </c>
       <c r="L19" s="3">
-        <v>202</v>
+        <v>92</v>
       </c>
       <c r="M19" s="3">
-        <v>233</v>
+        <v>94</v>
       </c>
       <c r="N19" s="3">
-        <v>157</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B20" s="3">
-        <v>14</v>
+        <v>283</v>
       </c>
       <c r="C20" s="3">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D20" s="3">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E20" s="3">
-        <v>2</v>
-      </c>
-      <c r="F20" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="F20" s="3">
+        <v>16</v>
+      </c>
       <c r="G20" s="3">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="H20" s="3">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I20" s="3">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="J20" s="3">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="K20" s="3">
-        <v>1</v>
-      </c>
-      <c r="L20" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="L20" s="3">
+        <v>36</v>
+      </c>
       <c r="M20" s="3">
-        <v>4</v>
-      </c>
-      <c r="N20" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="N20" s="3">
+        <v>28</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B21" s="3">
-        <v>1010</v>
+        <v>80</v>
       </c>
       <c r="C21" s="3">
-        <v>118</v>
+        <v>7</v>
       </c>
       <c r="D21" s="3">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="E21" s="3">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="F21" s="3">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="G21" s="3">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="H21" s="3">
-        <v>118</v>
+        <v>7</v>
       </c>
       <c r="I21" s="3">
-        <v>103</v>
+        <v>5</v>
       </c>
       <c r="J21" s="3">
-        <v>83</v>
+        <v>13</v>
       </c>
       <c r="K21" s="3">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="L21" s="3">
-        <v>92</v>
+        <v>8</v>
       </c>
       <c r="M21" s="3">
-        <v>94</v>
+        <v>3</v>
       </c>
       <c r="N21" s="3">
-        <v>66</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22" s="3">
-        <v>283</v>
+        <v>15</v>
       </c>
       <c r="C22" s="3">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D22" s="3">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E22" s="3">
-        <v>17</v>
-      </c>
-      <c r="F22" s="3">
-        <v>16</v>
-      </c>
-      <c r="G22" s="3">
-        <v>27</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
       <c r="H22" s="3">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="I22" s="3">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="J22" s="3">
-        <v>16</v>
-      </c>
-      <c r="K22" s="3">
-        <v>36</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="K22" s="1"/>
       <c r="L22" s="3">
-        <v>36</v>
-      </c>
-      <c r="M22" s="3">
-        <v>32</v>
-      </c>
-      <c r="N22" s="3">
-        <v>28</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B23" s="3">
-        <v>80</v>
+        <v>246</v>
       </c>
       <c r="C23" s="3">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D23" s="3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E23" s="3">
+        <v>13</v>
+      </c>
+      <c r="F23" s="3">
         <v>10</v>
       </c>
-      <c r="F23" s="3">
-        <v>3</v>
-      </c>
       <c r="G23" s="3">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H23" s="3">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="I23" s="3">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="J23" s="3">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="K23" s="3">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="L23" s="3">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="M23" s="3">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="N23" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B24" s="3">
-        <v>15</v>
+        <v>10037</v>
       </c>
       <c r="C24" s="3">
-        <v>2</v>
+        <v>912</v>
       </c>
       <c r="D24" s="3">
-        <v>1</v>
+        <v>791</v>
       </c>
       <c r="E24" s="3">
-        <v>1</v>
-      </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+        <v>726</v>
+      </c>
+      <c r="F24" s="3">
+        <v>649</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1012</v>
+      </c>
       <c r="H24" s="3">
-        <v>3</v>
+        <v>1040</v>
       </c>
       <c r="I24" s="3">
-        <v>2</v>
+        <v>1064</v>
       </c>
       <c r="J24" s="3">
-        <v>5</v>
-      </c>
-      <c r="K24" s="1"/>
+        <v>635</v>
+      </c>
+      <c r="K24" s="3">
+        <v>558</v>
+      </c>
       <c r="L24" s="3">
-        <v>1</v>
-      </c>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
+        <v>754</v>
+      </c>
+      <c r="M24" s="3">
+        <v>1009</v>
+      </c>
+      <c r="N24" s="3">
+        <v>887</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B25" s="3">
-        <v>246</v>
+        <v>336</v>
       </c>
       <c r="C25" s="3">
+        <v>25</v>
+      </c>
+      <c r="D25" s="3">
+        <v>24</v>
+      </c>
+      <c r="E25" s="3">
+        <v>47</v>
+      </c>
+      <c r="F25" s="3">
+        <v>26</v>
+      </c>
+      <c r="G25" s="3">
+        <v>29</v>
+      </c>
+      <c r="H25" s="3">
+        <v>41</v>
+      </c>
+      <c r="I25" s="3">
+        <v>18</v>
+      </c>
+      <c r="J25" s="3">
+        <v>19</v>
+      </c>
+      <c r="K25" s="3">
+        <v>30</v>
+      </c>
+      <c r="L25" s="3">
+        <v>39</v>
+      </c>
+      <c r="M25" s="3">
+        <v>24</v>
+      </c>
+      <c r="N25" s="3">
         <v>14</v>
-      </c>
-      <c r="D25" s="3">
-        <v>10</v>
-      </c>
-      <c r="E25" s="3">
-        <v>13</v>
-      </c>
-      <c r="F25" s="3">
-        <v>10</v>
-      </c>
-      <c r="G25" s="3">
-        <v>20</v>
-      </c>
-      <c r="H25" s="3">
-        <v>23</v>
-      </c>
-      <c r="I25" s="3">
-        <v>28</v>
-      </c>
-      <c r="J25" s="3">
-        <v>24</v>
-      </c>
-      <c r="K25" s="3">
-        <v>28</v>
-      </c>
-      <c r="L25" s="3">
-        <v>29</v>
-      </c>
-      <c r="M25" s="3">
-        <v>31</v>
-      </c>
-      <c r="N25" s="3">
-        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26" s="3">
-        <v>10037</v>
+        <v>1511</v>
       </c>
       <c r="C26" s="3">
-        <v>912</v>
+        <v>101</v>
       </c>
       <c r="D26" s="3">
-        <v>791</v>
+        <v>107</v>
       </c>
       <c r="E26" s="3">
-        <v>726</v>
+        <v>128</v>
       </c>
       <c r="F26" s="3">
-        <v>649</v>
+        <v>114</v>
       </c>
       <c r="G26" s="3">
-        <v>1012</v>
+        <v>126</v>
       </c>
       <c r="H26" s="3">
-        <v>1040</v>
+        <v>140</v>
       </c>
       <c r="I26" s="3">
-        <v>1064</v>
+        <v>133</v>
       </c>
       <c r="J26" s="3">
-        <v>635</v>
+        <v>152</v>
       </c>
       <c r="K26" s="3">
-        <v>558</v>
+        <v>125</v>
       </c>
       <c r="L26" s="3">
-        <v>754</v>
+        <v>112</v>
       </c>
       <c r="M26" s="3">
-        <v>1009</v>
+        <v>164</v>
       </c>
       <c r="N26" s="3">
-        <v>887</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27" s="3">
-        <v>336</v>
-      </c>
-      <c r="C27" s="3">
-        <v>25</v>
-      </c>
-      <c r="D27" s="3">
-        <v>24</v>
-      </c>
-      <c r="E27" s="3">
-        <v>47</v>
-      </c>
-      <c r="F27" s="3">
-        <v>26</v>
-      </c>
-      <c r="G27" s="3">
-        <v>29</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
       <c r="H27" s="3">
-        <v>41</v>
-      </c>
-      <c r="I27" s="3">
-        <v>18</v>
-      </c>
-      <c r="J27" s="3">
-        <v>19</v>
-      </c>
-      <c r="K27" s="3">
-        <v>30</v>
-      </c>
-      <c r="L27" s="3">
-        <v>39</v>
-      </c>
-      <c r="M27" s="3">
-        <v>24</v>
-      </c>
-      <c r="N27" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="3">
-        <v>1511</v>
-      </c>
-      <c r="C28" s="3">
-        <v>101</v>
-      </c>
-      <c r="D28" s="3">
-        <v>107</v>
-      </c>
-      <c r="E28" s="3">
-        <v>128</v>
-      </c>
-      <c r="F28" s="3">
-        <v>114</v>
-      </c>
-      <c r="G28" s="3">
-        <v>126</v>
-      </c>
-      <c r="H28" s="3">
-        <v>140</v>
-      </c>
-      <c r="I28" s="3">
-        <v>133</v>
-      </c>
-      <c r="J28" s="3">
-        <v>152</v>
-      </c>
-      <c r="K28" s="3">
-        <v>125</v>
-      </c>
-      <c r="L28" s="3">
-        <v>112</v>
-      </c>
-      <c r="M28" s="3">
-        <v>164</v>
-      </c>
-      <c r="N28" s="3">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="3">
         <v>1</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="3">
-        <v>1</v>
-      </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1808,6 +1711,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="eDocument" ma:contentTypeID="0x0101000BC94875665D404BB1351B53C41FD2C000E5CBA74D75A77049B177D97877D56E03" ma:contentTypeVersion="55" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="849aa1d06b04c28173376e708035b9cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f94102a1-1d6c-4502-ac27-91905b9321dd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="26a80217159fa0c72fe0406038957729" ns2:_="">
     <xsd:import namespace="f94102a1-1d6c-4502-ac27-91905b9321dd"/>
@@ -2016,15 +1928,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2065,6 +1968,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D3B01A4-23B1-49D9-8623-8C86F318FB2A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D748ACE5-DACD-49AC-90BF-A6E917447A40}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2078,14 +1989,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D3B01A4-23B1-49D9-8623-8C86F318FB2A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>